<commit_message>
simulations for the preprint
</commit_message>
<xml_diff>
--- a/CommunityModeling/CommFitting/data/Jeffs_data/metabolomics/8-19-22 Metabolomics TMS Panel EC_PF_acetate.xlsx
+++ b/CommunityModeling/CommFitting/data/Jeffs_data/metabolomics/8-19-22 Metabolomics TMS Panel EC_PF_acetate.xlsx
@@ -760,10 +760,10 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -11563,10 +11563,10 @@
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F34" s="2"/>
+      <c r="F34" s="3"/>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
@@ -11765,7 +11765,7 @@
       <c r="C39">
         <v>0.34</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="2">
         <v>1.64</v>
       </c>
       <c r="E39" s="1">

</xml_diff>